<commit_message>
made about half the card ID's static variables
</commit_message>
<xml_diff>
--- a/Card ID table.xlsx
+++ b/Card ID table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="2556" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
apparently I changed the card ID table?
</commit_message>
<xml_diff>
--- a/Card ID table.xlsx
+++ b/Card ID table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="2556" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>